<commit_message>
03 html/js lista 02 finish
</commit_message>
<xml_diff>
--- a/Pasta1.xlsx
+++ b/Pasta1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Backup\Cursos\SantanderCODES\Curso FrontEnd - Fase 3 - Turma 1004\02-Logica_de_Programacao_I_JS-TS\Exercícios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D7FA2C-6E83-4D93-AC98-9DA0B1731D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE53CA9-48B2-4EBD-837B-A3B87B1F1889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{890533D9-3878-406F-84C8-A9C22679028A}"/>
   </bookViews>
@@ -2568,8 +2568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F621F675-606C-4E6C-9645-C5CCA0CCB313}">
   <dimension ref="A1:F198"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2578,7 +2578,7 @@
     <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="105.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="196.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2608,8 +2608,8 @@
         <v>&lt;option value="Afeganistão"&gt;Afeganistão&lt;/option&gt;</v>
       </c>
       <c r="E2" t="str">
-        <f>"case '"&amp;A2&amp;"':"&amp;"mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;"</f>
-        <v>case 'Afeganistão':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <f>"case '"&amp;A2&amp;"':"&amp;"mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;"</f>
+        <v>case 'Afeganistão':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F2" t="str">
         <f>""""&amp;A2&amp;""": """&amp;B2&amp;""","""&amp;B2&amp;""":"""&amp;C2&amp;""","</f>
@@ -2631,8 +2631,8 @@
         <v>&lt;option value="África do Sul"&gt;África do Sul&lt;/option&gt;</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E66" si="1">"case '"&amp;A3&amp;"':"&amp;"mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;"</f>
-        <v>case 'África do Sul':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <f t="shared" ref="E3:E66" si="1">"case '"&amp;A3&amp;"':"&amp;"mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;"</f>
+        <v>case 'África do Sul':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F66" si="2">""""&amp;A3&amp;""": """&amp;B3&amp;""","""&amp;B3&amp;""":"""&amp;C3&amp;""","</f>
@@ -2655,7 +2655,7 @@
       </c>
       <c r="E4" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Albânia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Albânia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="2"/>
@@ -2678,7 +2678,7 @@
       </c>
       <c r="E5" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Alemanha':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Alemanha':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="2"/>
@@ -2701,7 +2701,7 @@
       </c>
       <c r="E6" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Andorra':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Andorra':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="2"/>
@@ -2724,7 +2724,7 @@
       </c>
       <c r="E7" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Angola':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Angola':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="2"/>
@@ -2747,7 +2747,7 @@
       </c>
       <c r="E8" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Antiga e Barbuda':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Antiga e Barbuda':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="2"/>
@@ -2770,7 +2770,7 @@
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Arábia Saudita':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Arábia Saudita':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="2"/>
@@ -2793,7 +2793,7 @@
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Argélia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Argélia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="2"/>
@@ -2816,7 +2816,7 @@
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Argentina':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Argentina':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="2"/>
@@ -2839,7 +2839,7 @@
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Arménia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Arménia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="2"/>
@@ -2862,7 +2862,7 @@
       </c>
       <c r="E13" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Austrália':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Austrália':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="2"/>
@@ -2885,7 +2885,7 @@
       </c>
       <c r="E14" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Áustria':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Áustria':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="2"/>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="E15" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Azerbaijão':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Azerbaijão':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="2"/>
@@ -2931,7 +2931,7 @@
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Bahamas':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Bahamas':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="2"/>
@@ -2954,7 +2954,7 @@
       </c>
       <c r="E17" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Bangladexe':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Bangladexe':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="2"/>
@@ -2977,7 +2977,7 @@
       </c>
       <c r="E18" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Barbados':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Barbados':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="2"/>
@@ -3000,7 +3000,7 @@
       </c>
       <c r="E19" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Barém':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Barém':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="2"/>
@@ -3023,7 +3023,7 @@
       </c>
       <c r="E20" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Bélgica':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Bélgica':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="2"/>
@@ -3046,7 +3046,7 @@
       </c>
       <c r="E21" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Belize':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Belize':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="2"/>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="E22" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Benim':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Benim':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="2"/>
@@ -3092,7 +3092,7 @@
       </c>
       <c r="E23" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Bielorrússia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Bielorrússia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="2"/>
@@ -3115,7 +3115,7 @@
       </c>
       <c r="E24" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Bolívia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Bolívia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="2"/>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="E25" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Bósnia e Herzegovina':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Bósnia e Herzegovina':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="2"/>
@@ -3161,7 +3161,7 @@
       </c>
       <c r="E26" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Botsuana':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Botsuana':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="2"/>
@@ -3184,7 +3184,7 @@
       </c>
       <c r="E27" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Brasil':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Brasil':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="2"/>
@@ -3207,7 +3207,7 @@
       </c>
       <c r="E28" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Brunei':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Brunei':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="2"/>
@@ -3230,7 +3230,7 @@
       </c>
       <c r="E29" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Bulgária':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Bulgária':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="2"/>
@@ -3253,7 +3253,7 @@
       </c>
       <c r="E30" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Burquina Faso':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Burquina Faso':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="2"/>
@@ -3276,7 +3276,7 @@
       </c>
       <c r="E31" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Burúndi':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Burúndi':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="2"/>
@@ -3299,7 +3299,7 @@
       </c>
       <c r="E32" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Butão':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Butão':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="2"/>
@@ -3322,7 +3322,7 @@
       </c>
       <c r="E33" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Cabo Verde':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Cabo Verde':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="2"/>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="E34" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Camarões':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Camarões':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="2"/>
@@ -3368,7 +3368,7 @@
       </c>
       <c r="E35" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Camboja':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Camboja':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="2"/>
@@ -3391,7 +3391,7 @@
       </c>
       <c r="E36" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Canadá':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Canadá':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="2"/>
@@ -3414,7 +3414,7 @@
       </c>
       <c r="E37" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Catar':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Catar':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="2"/>
@@ -3437,7 +3437,7 @@
       </c>
       <c r="E38" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Cazaquistão':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Cazaquistão':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="2"/>
@@ -3460,7 +3460,7 @@
       </c>
       <c r="E39" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Chade':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Chade':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="2"/>
@@ -3483,7 +3483,7 @@
       </c>
       <c r="E40" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Chile':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Chile':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="2"/>
@@ -3506,7 +3506,7 @@
       </c>
       <c r="E41" t="str">
         <f t="shared" si="1"/>
-        <v>case 'China':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'China':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="2"/>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="E42" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Chipre':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Chipre':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="2"/>
@@ -3552,7 +3552,7 @@
       </c>
       <c r="E43" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Colômbia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Colômbia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="2"/>
@@ -3575,7 +3575,7 @@
       </c>
       <c r="E44" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Comores':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Comores':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="2"/>
@@ -3598,7 +3598,7 @@
       </c>
       <c r="E45" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Congo-Brazzaville':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Congo-Brazzaville':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="2"/>
@@ -3621,7 +3621,7 @@
       </c>
       <c r="E46" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Coreia do Norte':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Coreia do Norte':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="2"/>
@@ -3644,7 +3644,7 @@
       </c>
       <c r="E47" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Coreia do Sul':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Coreia do Sul':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="2"/>
@@ -3667,7 +3667,7 @@
       </c>
       <c r="E48" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Cosovo':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Cosovo':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="2"/>
@@ -3690,7 +3690,7 @@
       </c>
       <c r="E49" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Costa do Marfim':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Costa do Marfim':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" si="2"/>
@@ -3713,7 +3713,7 @@
       </c>
       <c r="E50" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Costa Rica':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Costa Rica':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" si="2"/>
@@ -3736,7 +3736,7 @@
       </c>
       <c r="E51" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Croácia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Croácia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="2"/>
@@ -3759,7 +3759,7 @@
       </c>
       <c r="E52" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Cuaite':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Cuaite':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="2"/>
@@ -3782,7 +3782,7 @@
       </c>
       <c r="E53" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Cuba':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Cuba':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F53" t="str">
         <f t="shared" si="2"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="E54" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Dinamarca':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Dinamarca':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="2"/>
@@ -3828,7 +3828,7 @@
       </c>
       <c r="E55" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Dominica':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Dominica':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F55" t="str">
         <f t="shared" si="2"/>
@@ -3851,7 +3851,7 @@
       </c>
       <c r="E56" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Egito':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Egito':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="2"/>
@@ -3874,7 +3874,7 @@
       </c>
       <c r="E57" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Emirados Árabes Unidos':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Emirados Árabes Unidos':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="2"/>
@@ -3897,7 +3897,7 @@
       </c>
       <c r="E58" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Equador':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Equador':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="2"/>
@@ -3920,7 +3920,7 @@
       </c>
       <c r="E59" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Eritreia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Eritreia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F59" t="str">
         <f t="shared" si="2"/>
@@ -3943,7 +3943,7 @@
       </c>
       <c r="E60" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Eslováquia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Eslováquia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F60" t="str">
         <f t="shared" si="2"/>
@@ -3966,7 +3966,7 @@
       </c>
       <c r="E61" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Eslovénia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Eslovénia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F61" t="str">
         <f t="shared" si="2"/>
@@ -3989,7 +3989,7 @@
       </c>
       <c r="E62" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Espanha':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Espanha':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F62" t="str">
         <f t="shared" si="2"/>
@@ -4012,7 +4012,7 @@
       </c>
       <c r="E63" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Essuatíni':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Essuatíni':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F63" t="str">
         <f t="shared" si="2"/>
@@ -4035,7 +4035,7 @@
       </c>
       <c r="E64" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Estado da Palestina':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Estado da Palestina':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F64" t="str">
         <f t="shared" si="2"/>
@@ -4058,7 +4058,7 @@
       </c>
       <c r="E65" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Estados Unidos':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Estados Unidos':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F65" t="str">
         <f t="shared" si="2"/>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="E66" t="str">
         <f t="shared" si="1"/>
-        <v>case 'Estónia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Estónia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F66" t="str">
         <f t="shared" si="2"/>
@@ -4103,8 +4103,8 @@
         <v>&lt;option value="Etiópia"&gt;Etiópia&lt;/option&gt;</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E130" si="4">"case '"&amp;A67&amp;"':"&amp;"mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;"</f>
-        <v>case 'Etiópia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <f t="shared" ref="E67:E130" si="4">"case '"&amp;A67&amp;"':"&amp;"mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;"</f>
+        <v>case 'Etiópia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F67" t="str">
         <f t="shared" ref="F67:F130" si="5">""""&amp;A67&amp;""": """&amp;B67&amp;""","""&amp;B67&amp;""":"""&amp;C67&amp;""","</f>
@@ -4127,7 +4127,7 @@
       </c>
       <c r="E68" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Fiji':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Fiji':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F68" t="str">
         <f t="shared" si="5"/>
@@ -4150,7 +4150,7 @@
       </c>
       <c r="E69" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Filipinas':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Filipinas':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F69" t="str">
         <f t="shared" si="5"/>
@@ -4173,7 +4173,7 @@
       </c>
       <c r="E70" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Finlândia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Finlândia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F70" t="str">
         <f t="shared" si="5"/>
@@ -4196,7 +4196,7 @@
       </c>
       <c r="E71" t="str">
         <f t="shared" si="4"/>
-        <v>case 'França':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'França':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F71" t="str">
         <f t="shared" si="5"/>
@@ -4219,7 +4219,7 @@
       </c>
       <c r="E72" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Gabão':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Gabão':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F72" t="str">
         <f t="shared" si="5"/>
@@ -4242,7 +4242,7 @@
       </c>
       <c r="E73" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Gâmbia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Gâmbia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F73" t="str">
         <f t="shared" si="5"/>
@@ -4265,7 +4265,7 @@
       </c>
       <c r="E74" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Gana':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Gana':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F74" t="str">
         <f t="shared" si="5"/>
@@ -4288,7 +4288,7 @@
       </c>
       <c r="E75" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Geórgia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Geórgia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F75" t="str">
         <f t="shared" si="5"/>
@@ -4311,7 +4311,7 @@
       </c>
       <c r="E76" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Granada':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Granada':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F76" t="str">
         <f t="shared" si="5"/>
@@ -4334,7 +4334,7 @@
       </c>
       <c r="E77" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Grécia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Grécia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F77" t="str">
         <f t="shared" si="5"/>
@@ -4357,7 +4357,7 @@
       </c>
       <c r="E78" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Guatemala':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Guatemala':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F78" t="str">
         <f t="shared" si="5"/>
@@ -4380,7 +4380,7 @@
       </c>
       <c r="E79" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Guiana':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Guiana':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F79" t="str">
         <f t="shared" si="5"/>
@@ -4403,7 +4403,7 @@
       </c>
       <c r="E80" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Guiné':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Guiné':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F80" t="str">
         <f t="shared" si="5"/>
@@ -4426,7 +4426,7 @@
       </c>
       <c r="E81" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Guiné Equatorial':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Guiné Equatorial':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F81" t="str">
         <f t="shared" si="5"/>
@@ -4449,7 +4449,7 @@
       </c>
       <c r="E82" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Guiné-Bissau':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Guiné-Bissau':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F82" t="str">
         <f t="shared" si="5"/>
@@ -4472,7 +4472,7 @@
       </c>
       <c r="E83" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Haiti':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Haiti':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F83" t="str">
         <f t="shared" si="5"/>
@@ -4495,7 +4495,7 @@
       </c>
       <c r="E84" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Honduras':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Honduras':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F84" t="str">
         <f t="shared" si="5"/>
@@ -4518,7 +4518,7 @@
       </c>
       <c r="E85" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Hungria':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Hungria':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F85" t="str">
         <f t="shared" si="5"/>
@@ -4541,7 +4541,7 @@
       </c>
       <c r="E86" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Iémen':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Iémen':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F86" t="str">
         <f t="shared" si="5"/>
@@ -4564,7 +4564,7 @@
       </c>
       <c r="E87" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Ilhas Marechal':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Ilhas Marechal':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F87" t="str">
         <f t="shared" si="5"/>
@@ -4587,7 +4587,7 @@
       </c>
       <c r="E88" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Índia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Índia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F88" t="str">
         <f t="shared" si="5"/>
@@ -4610,7 +4610,7 @@
       </c>
       <c r="E89" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Indonésia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Indonésia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F89" t="str">
         <f t="shared" si="5"/>
@@ -4633,7 +4633,7 @@
       </c>
       <c r="E90" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Irão':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Irão':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F90" t="str">
         <f t="shared" si="5"/>
@@ -4656,7 +4656,7 @@
       </c>
       <c r="E91" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Iraque':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Iraque':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F91" t="str">
         <f t="shared" si="5"/>
@@ -4679,7 +4679,7 @@
       </c>
       <c r="E92" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Irlanda':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Irlanda':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F92" t="str">
         <f t="shared" si="5"/>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="E93" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Islândia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Islândia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F93" t="str">
         <f t="shared" si="5"/>
@@ -4725,7 +4725,7 @@
       </c>
       <c r="E94" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Israel':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Israel':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F94" t="str">
         <f t="shared" si="5"/>
@@ -4748,7 +4748,7 @@
       </c>
       <c r="E95" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Itália':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Itália':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F95" t="str">
         <f t="shared" si="5"/>
@@ -4771,7 +4771,7 @@
       </c>
       <c r="E96" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Jamaica':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Jamaica':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F96" t="str">
         <f t="shared" si="5"/>
@@ -4794,7 +4794,7 @@
       </c>
       <c r="E97" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Japão':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Japão':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F97" t="str">
         <f t="shared" si="5"/>
@@ -4817,7 +4817,7 @@
       </c>
       <c r="E98" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Jibuti':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Jibuti':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F98" t="str">
         <f t="shared" si="5"/>
@@ -4840,7 +4840,7 @@
       </c>
       <c r="E99" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Jordânia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Jordânia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F99" t="str">
         <f t="shared" si="5"/>
@@ -4863,7 +4863,7 @@
       </c>
       <c r="E100" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Laus':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Laus':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F100" t="str">
         <f t="shared" si="5"/>
@@ -4886,7 +4886,7 @@
       </c>
       <c r="E101" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Lesoto':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Lesoto':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F101" t="str">
         <f t="shared" si="5"/>
@@ -4909,7 +4909,7 @@
       </c>
       <c r="E102" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Letónia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Letónia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F102" t="str">
         <f t="shared" si="5"/>
@@ -4932,7 +4932,7 @@
       </c>
       <c r="E103" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Líbano':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Líbano':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F103" t="str">
         <f t="shared" si="5"/>
@@ -4955,7 +4955,7 @@
       </c>
       <c r="E104" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Libéria':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Libéria':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F104" t="str">
         <f t="shared" si="5"/>
@@ -4978,7 +4978,7 @@
       </c>
       <c r="E105" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Líbia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Líbia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F105" t="str">
         <f t="shared" si="5"/>
@@ -5001,7 +5001,7 @@
       </c>
       <c r="E106" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Listenstaine':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Listenstaine':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F106" t="str">
         <f t="shared" si="5"/>
@@ -5024,7 +5024,7 @@
       </c>
       <c r="E107" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Lituânia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Lituânia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F107" t="str">
         <f t="shared" si="5"/>
@@ -5047,7 +5047,7 @@
       </c>
       <c r="E108" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Luxemburgo':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Luxemburgo':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F108" t="str">
         <f t="shared" si="5"/>
@@ -5070,7 +5070,7 @@
       </c>
       <c r="E109" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Macedónia do Norte':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Macedónia do Norte':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F109" t="str">
         <f t="shared" si="5"/>
@@ -5093,7 +5093,7 @@
       </c>
       <c r="E110" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Madagáscar':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Madagáscar':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F110" t="str">
         <f t="shared" si="5"/>
@@ -5116,7 +5116,7 @@
       </c>
       <c r="E111" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Malásia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Malásia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F111" t="str">
         <f t="shared" si="5"/>
@@ -5139,7 +5139,7 @@
       </c>
       <c r="E112" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Maláui':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Maláui':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F112" t="str">
         <f t="shared" si="5"/>
@@ -5162,7 +5162,7 @@
       </c>
       <c r="E113" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Maldivas':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Maldivas':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F113" t="str">
         <f t="shared" si="5"/>
@@ -5185,7 +5185,7 @@
       </c>
       <c r="E114" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Mali':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Mali':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F114" t="str">
         <f t="shared" si="5"/>
@@ -5208,7 +5208,7 @@
       </c>
       <c r="E115" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Malta':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Malta':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F115" t="str">
         <f t="shared" si="5"/>
@@ -5231,7 +5231,7 @@
       </c>
       <c r="E116" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Marrocos':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Marrocos':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F116" t="str">
         <f t="shared" si="5"/>
@@ -5254,7 +5254,7 @@
       </c>
       <c r="E117" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Maurícia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Maurícia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F117" t="str">
         <f t="shared" si="5"/>
@@ -5277,7 +5277,7 @@
       </c>
       <c r="E118" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Mauritânia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Mauritânia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F118" t="str">
         <f t="shared" si="5"/>
@@ -5300,7 +5300,7 @@
       </c>
       <c r="E119" t="str">
         <f t="shared" si="4"/>
-        <v>case 'México':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'México':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F119" t="str">
         <f t="shared" si="5"/>
@@ -5323,7 +5323,7 @@
       </c>
       <c r="E120" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Mianmar':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Mianmar':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F120" t="str">
         <f t="shared" si="5"/>
@@ -5346,7 +5346,7 @@
       </c>
       <c r="E121" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Micronésia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Micronésia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F121" t="str">
         <f t="shared" si="5"/>
@@ -5369,7 +5369,7 @@
       </c>
       <c r="E122" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Moçambique':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Moçambique':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F122" t="str">
         <f t="shared" si="5"/>
@@ -5392,7 +5392,7 @@
       </c>
       <c r="E123" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Moldávia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Moldávia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F123" t="str">
         <f t="shared" si="5"/>
@@ -5415,7 +5415,7 @@
       </c>
       <c r="E124" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Mónaco':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Mónaco':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F124" t="str">
         <f t="shared" si="5"/>
@@ -5438,7 +5438,7 @@
       </c>
       <c r="E125" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Mongólia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Mongólia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F125" t="str">
         <f t="shared" si="5"/>
@@ -5461,7 +5461,7 @@
       </c>
       <c r="E126" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Montenegro':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Montenegro':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F126" t="str">
         <f t="shared" si="5"/>
@@ -5484,7 +5484,7 @@
       </c>
       <c r="E127" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Namíbia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Namíbia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F127" t="str">
         <f t="shared" si="5"/>
@@ -5507,7 +5507,7 @@
       </c>
       <c r="E128" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Nauru':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Nauru':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F128" t="str">
         <f t="shared" si="5"/>
@@ -5530,7 +5530,7 @@
       </c>
       <c r="E129" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Nepal':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Nepal':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F129" t="str">
         <f t="shared" si="5"/>
@@ -5553,7 +5553,7 @@
       </c>
       <c r="E130" t="str">
         <f t="shared" si="4"/>
-        <v>case 'Nicarágua':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Nicarágua':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F130" t="str">
         <f t="shared" si="5"/>
@@ -5575,8 +5575,8 @@
         <v>&lt;option value="Níger"&gt;Níger&lt;/option&gt;</v>
       </c>
       <c r="E131" t="str">
-        <f t="shared" ref="E131:E194" si="7">"case '"&amp;A131&amp;"':"&amp;"mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;"</f>
-        <v>case 'Níger':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <f t="shared" ref="E131:E194" si="7">"case '"&amp;A131&amp;"':"&amp;"mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;"</f>
+        <v>case 'Níger':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F131" t="str">
         <f t="shared" ref="F131:F194" si="8">""""&amp;A131&amp;""": """&amp;B131&amp;""","""&amp;B131&amp;""":"""&amp;C131&amp;""","</f>
@@ -5599,7 +5599,7 @@
       </c>
       <c r="E132" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Nigéria':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Nigéria':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F132" t="str">
         <f t="shared" si="8"/>
@@ -5622,7 +5622,7 @@
       </c>
       <c r="E133" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Noruega':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Noruega':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F133" t="str">
         <f t="shared" si="8"/>
@@ -5645,7 +5645,7 @@
       </c>
       <c r="E134" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Nova Zelândia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Nova Zelândia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F134" t="str">
         <f t="shared" si="8"/>
@@ -5668,7 +5668,7 @@
       </c>
       <c r="E135" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Omã':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Omã':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F135" t="str">
         <f t="shared" si="8"/>
@@ -5691,7 +5691,7 @@
       </c>
       <c r="E136" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Países Baixos':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Países Baixos':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F136" t="str">
         <f t="shared" si="8"/>
@@ -5714,7 +5714,7 @@
       </c>
       <c r="E137" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Palau':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Palau':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F137" t="str">
         <f t="shared" si="8"/>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="E138" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Panamá':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Panamá':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F138" t="str">
         <f t="shared" si="8"/>
@@ -5760,7 +5760,7 @@
       </c>
       <c r="E139" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Papua Nova Guiné':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Papua Nova Guiné':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F139" t="str">
         <f t="shared" si="8"/>
@@ -5783,7 +5783,7 @@
       </c>
       <c r="E140" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Paquistão':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Paquistão':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F140" t="str">
         <f t="shared" si="8"/>
@@ -5806,7 +5806,7 @@
       </c>
       <c r="E141" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Paraguai':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Paraguai':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F141" t="str">
         <f t="shared" si="8"/>
@@ -5829,7 +5829,7 @@
       </c>
       <c r="E142" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Peru':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Peru':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F142" t="str">
         <f t="shared" si="8"/>
@@ -5852,7 +5852,7 @@
       </c>
       <c r="E143" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Polónia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Polónia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F143" t="str">
         <f t="shared" si="8"/>
@@ -5875,7 +5875,7 @@
       </c>
       <c r="E144" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Portugal':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Portugal':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F144" t="str">
         <f t="shared" si="8"/>
@@ -5898,7 +5898,7 @@
       </c>
       <c r="E145" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Quénia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Quénia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F145" t="str">
         <f t="shared" si="8"/>
@@ -5921,7 +5921,7 @@
       </c>
       <c r="E146" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Quirguistão':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Quirguistão':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F146" t="str">
         <f t="shared" si="8"/>
@@ -5944,7 +5944,7 @@
       </c>
       <c r="E147" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Quiribáti':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Quiribáti':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F147" t="str">
         <f t="shared" si="8"/>
@@ -5967,7 +5967,7 @@
       </c>
       <c r="E148" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Reino Unido':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Reino Unido':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F148" t="str">
         <f t="shared" si="8"/>
@@ -5990,7 +5990,7 @@
       </c>
       <c r="E149" t="str">
         <f t="shared" si="7"/>
-        <v>case 'República Centro-Africana':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'República Centro-Africana':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F149" t="str">
         <f t="shared" si="8"/>
@@ -6013,7 +6013,7 @@
       </c>
       <c r="E150" t="str">
         <f t="shared" si="7"/>
-        <v>case 'República Checa':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'República Checa':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F150" t="str">
         <f t="shared" si="8"/>
@@ -6036,7 +6036,7 @@
       </c>
       <c r="E151" t="str">
         <f t="shared" si="7"/>
-        <v>case 'República Democrática do Congo':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'República Democrática do Congo':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F151" t="str">
         <f t="shared" si="8"/>
@@ -6059,7 +6059,7 @@
       </c>
       <c r="E152" t="str">
         <f t="shared" si="7"/>
-        <v>case 'República Dominicana':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'República Dominicana':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F152" t="str">
         <f t="shared" si="8"/>
@@ -6082,7 +6082,7 @@
       </c>
       <c r="E153" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Roménia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Roménia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F153" t="str">
         <f t="shared" si="8"/>
@@ -6105,7 +6105,7 @@
       </c>
       <c r="E154" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Ruanda':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Ruanda':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F154" t="str">
         <f t="shared" si="8"/>
@@ -6128,7 +6128,7 @@
       </c>
       <c r="E155" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Rússia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Rússia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F155" t="str">
         <f t="shared" si="8"/>
@@ -6151,7 +6151,7 @@
       </c>
       <c r="E156" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Salomão':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Salomão':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F156" t="str">
         <f t="shared" si="8"/>
@@ -6174,7 +6174,7 @@
       </c>
       <c r="E157" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Salvador':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Salvador':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F157" t="str">
         <f t="shared" si="8"/>
@@ -6197,7 +6197,7 @@
       </c>
       <c r="E158" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Samoa':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Samoa':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F158" t="str">
         <f t="shared" si="8"/>
@@ -6220,7 +6220,7 @@
       </c>
       <c r="E159" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Santa Lúcia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Santa Lúcia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F159" t="str">
         <f t="shared" si="8"/>
@@ -6243,7 +6243,7 @@
       </c>
       <c r="E160" t="str">
         <f t="shared" si="7"/>
-        <v>case 'São Cristóvão e Neves':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'São Cristóvão e Neves':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F160" t="str">
         <f t="shared" si="8"/>
@@ -6266,7 +6266,7 @@
       </c>
       <c r="E161" t="str">
         <f t="shared" si="7"/>
-        <v>case 'São Marinho':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'São Marinho':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F161" t="str">
         <f t="shared" si="8"/>
@@ -6289,7 +6289,7 @@
       </c>
       <c r="E162" t="str">
         <f t="shared" si="7"/>
-        <v>case 'São Tomé e Príncipe':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'São Tomé e Príncipe':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F162" t="str">
         <f t="shared" si="8"/>
@@ -6312,7 +6312,7 @@
       </c>
       <c r="E163" t="str">
         <f t="shared" si="7"/>
-        <v>case 'São Vicente e Granadinas':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'São Vicente e Granadinas':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F163" t="str">
         <f t="shared" si="8"/>
@@ -6335,7 +6335,7 @@
       </c>
       <c r="E164" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Seicheles':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Seicheles':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F164" t="str">
         <f t="shared" si="8"/>
@@ -6358,7 +6358,7 @@
       </c>
       <c r="E165" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Senegal':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Senegal':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F165" t="str">
         <f t="shared" si="8"/>
@@ -6381,7 +6381,7 @@
       </c>
       <c r="E166" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Serra Leoa':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Serra Leoa':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F166" t="str">
         <f t="shared" si="8"/>
@@ -6404,7 +6404,7 @@
       </c>
       <c r="E167" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Sérvia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Sérvia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F167" t="str">
         <f t="shared" si="8"/>
@@ -6427,7 +6427,7 @@
       </c>
       <c r="E168" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Singapura':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Singapura':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F168" t="str">
         <f t="shared" si="8"/>
@@ -6450,7 +6450,7 @@
       </c>
       <c r="E169" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Síria':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Síria':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F169" t="str">
         <f t="shared" si="8"/>
@@ -6473,7 +6473,7 @@
       </c>
       <c r="E170" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Somália':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Somália':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F170" t="str">
         <f t="shared" si="8"/>
@@ -6496,7 +6496,7 @@
       </c>
       <c r="E171" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Sri Lanca':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Sri Lanca':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F171" t="str">
         <f t="shared" si="8"/>
@@ -6519,7 +6519,7 @@
       </c>
       <c r="E172" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Sudão':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Sudão':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F172" t="str">
         <f t="shared" si="8"/>
@@ -6542,7 +6542,7 @@
       </c>
       <c r="E173" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Sudão do Sul':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Sudão do Sul':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F173" t="str">
         <f t="shared" si="8"/>
@@ -6565,7 +6565,7 @@
       </c>
       <c r="E174" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Suécia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Suécia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F174" t="str">
         <f t="shared" si="8"/>
@@ -6588,7 +6588,7 @@
       </c>
       <c r="E175" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Suíça':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Suíça':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F175" t="str">
         <f t="shared" si="8"/>
@@ -6611,7 +6611,7 @@
       </c>
       <c r="E176" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Suriname':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Suriname':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F176" t="str">
         <f t="shared" si="8"/>
@@ -6634,7 +6634,7 @@
       </c>
       <c r="E177" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Tailândia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Tailândia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F177" t="str">
         <f t="shared" si="8"/>
@@ -6657,7 +6657,7 @@
       </c>
       <c r="E178" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Taiuã':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Taiuã':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F178" t="str">
         <f t="shared" si="8"/>
@@ -6680,7 +6680,7 @@
       </c>
       <c r="E179" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Tajiquistão':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Tajiquistão':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F179" t="str">
         <f t="shared" si="8"/>
@@ -6703,7 +6703,7 @@
       </c>
       <c r="E180" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Tanzânia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Tanzânia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F180" t="str">
         <f t="shared" si="8"/>
@@ -6726,7 +6726,7 @@
       </c>
       <c r="E181" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Timor-Leste':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Timor-Leste':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F181" t="str">
         <f t="shared" si="8"/>
@@ -6749,7 +6749,7 @@
       </c>
       <c r="E182" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Togo':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Togo':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F182" t="str">
         <f t="shared" si="8"/>
@@ -6772,7 +6772,7 @@
       </c>
       <c r="E183" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Tonga':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Tonga':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F183" t="str">
         <f t="shared" si="8"/>
@@ -6795,7 +6795,7 @@
       </c>
       <c r="E184" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Trindade e Tobago':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Trindade e Tobago':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F184" t="str">
         <f t="shared" si="8"/>
@@ -6818,7 +6818,7 @@
       </c>
       <c r="E185" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Tunísia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Tunísia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F185" t="str">
         <f t="shared" si="8"/>
@@ -6841,7 +6841,7 @@
       </c>
       <c r="E186" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Turcomenistão':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Turcomenistão':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F186" t="str">
         <f t="shared" si="8"/>
@@ -6864,7 +6864,7 @@
       </c>
       <c r="E187" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Turquia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Turquia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F187" t="str">
         <f t="shared" si="8"/>
@@ -6887,7 +6887,7 @@
       </c>
       <c r="E188" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Tuvalu':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Tuvalu':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F188" t="str">
         <f t="shared" si="8"/>
@@ -6910,7 +6910,7 @@
       </c>
       <c r="E189" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Ucrânia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Ucrânia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F189" t="str">
         <f t="shared" si="8"/>
@@ -6933,7 +6933,7 @@
       </c>
       <c r="E190" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Uganda':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Uganda':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F190" t="str">
         <f t="shared" si="8"/>
@@ -6956,7 +6956,7 @@
       </c>
       <c r="E191" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Uruguai':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Uruguai':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F191" t="str">
         <f t="shared" si="8"/>
@@ -6979,7 +6979,7 @@
       </c>
       <c r="E192" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Usbequistão':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Usbequistão':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F192" t="str">
         <f t="shared" si="8"/>
@@ -7002,7 +7002,7 @@
       </c>
       <c r="E193" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Vanuatu':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Vanuatu':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F193" t="str">
         <f t="shared" si="8"/>
@@ -7025,7 +7025,7 @@
       </c>
       <c r="E194" t="str">
         <f t="shared" si="7"/>
-        <v>case 'Vaticano':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Vaticano':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F194" t="str">
         <f t="shared" si="8"/>
@@ -7047,8 +7047,8 @@
         <v>&lt;option value="Venezuela"&gt;Venezuela&lt;/option&gt;</v>
       </c>
       <c r="E195" t="str">
-        <f t="shared" ref="E195:E198" si="10">"case '"&amp;A195&amp;"':"&amp;"mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;"</f>
-        <v>case 'Venezuela':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <f t="shared" ref="E195:E198" si="10">"case '"&amp;A195&amp;"':"&amp;"mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;"</f>
+        <v>case 'Venezuela':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F195" t="str">
         <f t="shared" ref="F195:F213" si="11">""""&amp;A195&amp;""": """&amp;B195&amp;""","""&amp;B195&amp;""":"""&amp;C195&amp;""","</f>
@@ -7071,7 +7071,7 @@
       </c>
       <c r="E196" t="str">
         <f t="shared" si="10"/>
-        <v>case 'Vietname':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Vietname':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F196" t="str">
         <f t="shared" si="11"/>
@@ -7094,7 +7094,7 @@
       </c>
       <c r="E197" t="str">
         <f t="shared" si="10"/>
-        <v>case 'Zâmbia':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Zâmbia':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F197" t="str">
         <f t="shared" si="11"/>
@@ -7117,7 +7117,7 @@
       </c>
       <c r="E198" t="str">
         <f t="shared" si="10"/>
-        <v>case 'Zimbábue':mensagem = `A Capital de ${pais} é ${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente ${paises[paises[pais]]}`;Break;</v>
+        <v>case 'Zimbábue':mensagem = `A Capital de &lt;strong&gt;${pais}&lt;/strong&gt; é &lt;/strong&gt;${paises[pais]}&lt;br&gt;`;mensagem += `E estão localizadoos no continente &lt;strong&gt;${paises[paises[pais]]}&lt;/strong&gt;`;</v>
       </c>
       <c r="F198" t="str">
         <f t="shared" si="11"/>
@@ -7325,5 +7325,6 @@
     <hyperlink ref="A198" r:id="rId197" display="https://www.sport-histoire.fr/pt/Geografia/Africa/Zimbabue.php" xr:uid="{3EB63A64-9B85-480B-98A6-5055C36890F7}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId198"/>
 </worksheet>
 </file>
</xml_diff>